<commit_message>
testing and a few fixes of queuing [CAN-81] and exchange mailer [CAN-88] before deployment
</commit_message>
<xml_diff>
--- a/tests/testing_filepath/Phil305 F25/Phil305 F25 emails.xlsx
+++ b/tests/testing_filepath/Phil305 F25/Phil305 F25 emails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ars62917/Dropbox/CanvasHacks/tests/testing_output_folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ars62917/Dropbox/CanvasHacks/tests/testing_filepath/Phil305 F25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273EDC5F-FD90-FA4A-8B0E-203A5CD0D498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3180B058-913A-6844-8D41-DE2B40D29AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2560" yWindow="4320" windowWidth="27640" windowHeight="16940" xr2:uid="{91C7510D-43E0-034E-81D4-A3BCFDB6F5A5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="317">
   <si>
     <t>ID</t>
   </si>
@@ -976,7 +976,19 @@
     <t>Student, Test</t>
   </si>
   <si>
-    <t>test@test.com</t>
+    <t>beep, borp</t>
+  </si>
+  <si>
+    <t>borp, beep</t>
+  </si>
+  <si>
+    <t>adamswenson@gmail.com</t>
+  </si>
+  <si>
+    <t>aswenson@calstate.edu</t>
+  </si>
+  <si>
+    <t>nicomachus@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1255,6 +1267,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1739,20 +1752,32 @@
         <v>93</v>
       </c>
       <c r="D2" s="32" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="11" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="B3" s="11">
+        <v>169908</v>
+      </c>
       <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="D3" s="33" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B4" s="14">
+        <v>169957</v>
+      </c>
       <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="D4" s="31" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11"/>
@@ -2273,10 +2298,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{1C2919BE-7BD3-0241-AD54-329846D5C6C4}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{993EB384-E4B3-014F-A8DF-7B593287809A}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{B7554718-959E-3948-B104-6F92F9EC9FE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>